<commit_message>
meged svelte to master
</commit_message>
<xml_diff>
--- a/doc/UART машинка.xlsx
+++ b/doc/UART машинка.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Fuel cell\Car\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v.senichkin\Desktop\Projects\Car\SPITE-GUI\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Название 
 параметра</t>
@@ -146,12 +146,18 @@
   </si>
   <si>
     <t>1- разрядка 0-зарядка</t>
+  </si>
+  <si>
+    <t>Рекуперация</t>
+  </si>
+  <si>
+    <t>Вт*с</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -834,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,61 +1255,61 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="6">
-        <v>95</v>
-      </c>
-      <c r="E19" s="6">
-        <v>95</v>
-      </c>
-      <c r="F19" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v>5F</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="22"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="39">
-        <v>0</v>
-      </c>
-      <c r="E20" s="9">
-        <v>0</v>
-      </c>
-      <c r="F20" s="9" t="str">
-        <f t="shared" ref="F20" si="4">DEC2HEX(E20)</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="10">
-        <v>0</v>
-      </c>
-      <c r="I20" s="38" t="s">
-        <v>30</v>
+      <c r="B20" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="6">
+        <v>95</v>
+      </c>
+      <c r="E20" s="6">
+        <v>95</v>
+      </c>
+      <c r="F20" s="21" t="str">
+        <f t="shared" si="2"/>
+        <v>5F</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="7"/>
+      <c r="B21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="39">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9" t="str">
+        <f t="shared" ref="F21" si="4">DEC2HEX(E21)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -1415,6 +1421,29 @@
       <c r="I26" s="38" t="s">
         <v>39</v>
       </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>